<commit_message>
Update error table for import edit
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy (2) - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy (2) - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61014B5F-E215-43C5-B3D1-2E81BFD36F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47771F0E-F22C-4610-ABDE-5F91CC50BA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9655" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9654" uniqueCount="863">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5426,9 +5426,6 @@
   </si>
   <si>
     <t>197pm21905</t>
-  </si>
-  <si>
-    <t>hehe</t>
   </si>
 </sst>
 </file>
@@ -6352,7 +6349,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6520,9 +6517,7 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>863</v>
-      </c>
+      <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update show components for datatables when show lecturer error list
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy (2) - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy (2) - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6EC21B-EC3D-4881-83A3-2BC2CD6C549F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A7149-5932-4839-8028-BDBC56018D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5604" yWindow="3360" windowWidth="17172" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIÊU CHUẨN- phân công GV K28" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9654" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9655" uniqueCount="865">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5426,6 +5426,12 @@
   </si>
   <si>
     <t>197pm21905</t>
+  </si>
+  <si>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t>ehehe</t>
   </si>
 </sst>
 </file>
@@ -6346,10 +6352,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6612,7 +6618,7 @@
         <v>59</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>60</v>
@@ -6707,7 +6713,9 @@
       <c r="O4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>864</v>
+      </c>
       <c r="Q4" s="8" t="s">
         <v>60</v>
       </c>

</xml_diff>